<commit_message>
added origin map 2.0
</commit_message>
<xml_diff>
--- a/data/coronavirus_origin_data.xlsx
+++ b/data/coronavirus_origin_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\OneDrive\FYP2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C7CB53-7B4E-487E-B8AD-22FA16B38264}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE50AB3B-EDE1-4DBA-BF26-3CDF13AC78DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="788" xr2:uid="{BBD3DD9A-9B31-49E4-9DF5-3A64C89D46D5}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="1000" activeTab="5" xr2:uid="{BBD3DD9A-9B31-49E4-9DF5-3A64C89D46D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Lat-long (COVID-19)" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Lat-long (MERS)" sheetId="6" r:id="rId3"/>
     <sheet name="Lat-long (SARS)" sheetId="5" r:id="rId4"/>
     <sheet name="Connections (COVID-19)" sheetId="1" r:id="rId5"/>
-    <sheet name="North America" sheetId="2" r:id="rId6"/>
+    <sheet name="Connections (with lat_long)" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="250">
   <si>
     <t>Italy</t>
   </si>
@@ -774,6 +774,18 @@
   </si>
   <si>
     <t>Yemen</t>
+  </si>
+  <si>
+    <t>dest_lat</t>
+  </si>
+  <si>
+    <t>dest_long</t>
+  </si>
+  <si>
+    <t>origin_lat</t>
+  </si>
+  <si>
+    <t>origin_long</t>
   </si>
 </sst>
 </file>
@@ -815,9 +827,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1144,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8423BF-B94D-4FF8-B5CF-315498357D9F}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,16 +1188,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>30.9756</v>
       </c>
       <c r="C2">
         <v>104.27070000000001</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>80796</v>
       </c>
       <c r="E2">
@@ -1231,16 +1242,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>36</v>
       </c>
       <c r="C5">
         <v>128</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>7869</v>
       </c>
       <c r="F5" t="s">
@@ -1342,7 +1353,7 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>2281</v>
       </c>
       <c r="F11" t="s">
@@ -1444,7 +1455,7 @@
       <c r="C17">
         <v>9</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>1966</v>
       </c>
       <c r="F17" t="s">
@@ -1546,7 +1557,7 @@
       <c r="C23">
         <v>12</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>12462</v>
       </c>
       <c r="F23" t="s">
@@ -1614,7 +1625,7 @@
       <c r="C27">
         <v>-4</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>2277</v>
       </c>
       <c r="F27" t="s">
@@ -1679,7 +1690,7 @@
       <c r="C31">
         <v>53</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>9000</v>
       </c>
       <c r="F31" t="s">
@@ -1688,7 +1699,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="B32">
         <v>33.854700000000001</v>
@@ -2860,7 +2871,7 @@
       <c r="C101">
         <v>-95</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101" s="5">
         <v>1336</v>
       </c>
       <c r="F101" t="s">
@@ -3190,7 +3201,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="5"/>
+    <col min="4" max="5" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3203,13 +3214,13 @@
       <c r="C1" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3223,10 +3234,10 @@
       <c r="C2">
         <v>-9.4294986999999999</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>10675</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>4809</v>
       </c>
       <c r="F2" t="s">
@@ -3243,10 +3254,10 @@
       <c r="C3">
         <v>-11.7798891</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>14124</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>3956</v>
       </c>
       <c r="F3" t="s">
@@ -3263,10 +3274,10 @@
       <c r="C4">
         <v>-9.6966447999999996</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>3811</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>2543</v>
       </c>
       <c r="F4" t="s">
@@ -3283,10 +3294,10 @@
       <c r="C5">
         <v>8.6752768000000007</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>20</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>8</v>
       </c>
       <c r="F5" t="s">
@@ -3303,10 +3314,10 @@
       <c r="C6">
         <v>-3.9961660000000001</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>8</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>6</v>
       </c>
       <c r="F6" t="s">
@@ -3323,10 +3334,10 @@
       <c r="C7">
         <v>-89.401200000000003</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>4</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
       <c r="F7" t="s">
@@ -3343,10 +3354,10 @@
       <c r="C8">
         <v>9</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>0</v>
       </c>
       <c r="F8" t="s">
@@ -3363,10 +3374,10 @@
       <c r="C9">
         <v>-7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>0</v>
       </c>
       <c r="F9" t="s">
@@ -3383,10 +3394,10 @@
       <c r="C10">
         <v>-14.4523621</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0</v>
       </c>
       <c r="F10" t="s">
@@ -3403,10 +3414,10 @@
       <c r="C11">
         <v>-8</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>0</v>
       </c>
       <c r="F11" t="s">
@@ -3468,7 +3479,7 @@
       <c r="E2">
         <v>453</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3488,7 +3499,7 @@
       <c r="E3">
         <v>32</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3508,7 +3519,7 @@
       <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3528,7 +3539,7 @@
       <c r="E5">
         <v>6</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3548,7 +3559,7 @@
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3568,7 +3579,7 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3588,7 +3599,7 @@
       <c r="E8">
         <v>2</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3608,7 +3619,7 @@
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3628,7 +3639,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3648,7 +3659,7 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3668,7 +3679,7 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3688,7 +3699,7 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3708,7 +3719,7 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3728,7 +3739,7 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3748,7 +3759,7 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3768,7 +3779,7 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3788,7 +3799,7 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3808,7 +3819,7 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3828,7 +3839,7 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3848,7 +3859,7 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3868,7 +3879,7 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3888,7 +3899,7 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3908,7 +3919,7 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3928,7 +3939,7 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3948,7 +3959,7 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4000,7 +4011,7 @@
       <c r="C2">
         <v>104.195397</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>5327</v>
       </c>
       <c r="E2">
@@ -4020,7 +4031,7 @@
       <c r="C3">
         <v>114.109497</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>1755</v>
       </c>
       <c r="E3">
@@ -4560,8 +4571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D086343C-F872-446A-BD7D-B96E4ED95CA5}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection sqref="A1:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4569,7 +4580,7 @@
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4582,7 +4593,7 @@
       <c r="C1" t="s">
         <v>210</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
@@ -4599,7 +4610,7 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E2" t="s">
@@ -4616,7 +4627,7 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E3" t="s">
@@ -4633,7 +4644,7 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="E4" t="s">
@@ -4650,7 +4661,7 @@
       <c r="C5" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>43923</v>
       </c>
       <c r="E5" t="s">
@@ -4667,7 +4678,7 @@
       <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>43954</v>
       </c>
       <c r="E6" t="s">
@@ -4684,7 +4695,7 @@
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E7" t="s">
@@ -4701,7 +4712,7 @@
       <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>43833</v>
       </c>
       <c r="E8" t="s">
@@ -4718,7 +4729,7 @@
       <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E9" t="s">
@@ -4735,7 +4746,7 @@
       <c r="C10" t="s">
         <v>211</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>43924</v>
       </c>
       <c r="E10" t="s">
@@ -4752,7 +4763,7 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E11" t="s">
@@ -4769,7 +4780,7 @@
       <c r="C12" t="s">
         <v>224</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>84</v>
       </c>
       <c r="E12" t="s">
@@ -4786,7 +4797,7 @@
       <c r="C13" t="s">
         <v>224</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E13" t="s">
@@ -4803,7 +4814,7 @@
       <c r="C14" t="s">
         <v>224</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>86</v>
       </c>
       <c r="E14" t="s">
@@ -4820,7 +4831,7 @@
       <c r="C15" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E15" t="s">
@@ -4837,7 +4848,7 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>43924</v>
       </c>
       <c r="E16" t="s">
@@ -4854,7 +4865,7 @@
       <c r="C17" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>82</v>
       </c>
       <c r="E17" t="s">
@@ -4871,7 +4882,7 @@
       <c r="C18" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E18" t="s">
@@ -4888,7 +4899,7 @@
       <c r="C19" t="s">
         <v>224</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E19" t="s">
@@ -4905,7 +4916,7 @@
       <c r="C20" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>43864</v>
       </c>
       <c r="E20" t="s">
@@ -4922,7 +4933,7 @@
       <c r="C21" t="s">
         <v>211</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>43893</v>
       </c>
       <c r="E21" t="s">
@@ -4939,7 +4950,7 @@
       <c r="C22" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>82</v>
       </c>
       <c r="E22" t="s">
@@ -4956,7 +4967,7 @@
       <c r="C23" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E23" t="s">
@@ -4973,7 +4984,7 @@
       <c r="C24" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E24" t="s">
@@ -4990,7 +5001,7 @@
       <c r="C25" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E25" t="s">
@@ -5007,7 +5018,7 @@
       <c r="C26" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E26" t="s">
@@ -5024,7 +5035,7 @@
       <c r="C27" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E27" t="s">
@@ -5041,7 +5052,7 @@
       <c r="C28" t="s">
         <v>211</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>43924</v>
       </c>
       <c r="E28" t="s">
@@ -5058,7 +5069,7 @@
       <c r="C29" t="s">
         <v>211</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>43864</v>
       </c>
       <c r="E29" t="s">
@@ -5075,7 +5086,7 @@
       <c r="C30" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E30" t="s">
@@ -5092,7 +5103,7 @@
       <c r="C31" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E31" t="s">
@@ -5109,7 +5120,7 @@
       <c r="C32" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E32" t="s">
@@ -5126,7 +5137,7 @@
       <c r="C33" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>43954</v>
       </c>
       <c r="E33" t="s">
@@ -5143,7 +5154,7 @@
       <c r="C34" t="s">
         <v>211</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E34" t="s">
@@ -5160,7 +5171,7 @@
       <c r="C35" t="s">
         <v>224</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E35" t="s">
@@ -5177,7 +5188,7 @@
       <c r="C36" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E36" t="s">
@@ -5194,7 +5205,7 @@
       <c r="C37" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>43954</v>
       </c>
       <c r="E37" t="s">
@@ -5211,7 +5222,7 @@
       <c r="C38" t="s">
         <v>224</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E38" t="s">
@@ -5228,7 +5239,7 @@
       <c r="C39" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>43926</v>
       </c>
       <c r="E39" t="s">
@@ -5245,7 +5256,7 @@
       <c r="C40" t="s">
         <v>211</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>43864</v>
       </c>
       <c r="E40" t="s">
@@ -5262,7 +5273,7 @@
       <c r="C41" t="s">
         <v>211</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>43985</v>
       </c>
       <c r="E41" t="s">
@@ -5279,7 +5290,7 @@
       <c r="C42" t="s">
         <v>224</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>213</v>
       </c>
       <c r="E42" t="s">
@@ -5296,7 +5307,7 @@
       <c r="C43" t="s">
         <v>0</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>43864</v>
       </c>
       <c r="E43" t="s">
@@ -5313,7 +5324,7 @@
       <c r="C44" t="s">
         <v>0</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E44" t="s">
@@ -5330,7 +5341,7 @@
       <c r="C45" t="s">
         <v>211</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>43864</v>
       </c>
       <c r="E45" t="s">
@@ -5347,7 +5358,7 @@
       <c r="C46" t="s">
         <v>0</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>43954</v>
       </c>
       <c r="E46" t="s">
@@ -5364,7 +5375,7 @@
       <c r="C47" t="s">
         <v>211</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>43985</v>
       </c>
       <c r="E47" t="s">
@@ -5381,7 +5392,7 @@
       <c r="C48" t="s">
         <v>0</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>43864</v>
       </c>
       <c r="E48" t="s">
@@ -5398,7 +5409,7 @@
       <c r="C49" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E49" t="s">
@@ -5415,7 +5426,7 @@
       <c r="C50" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E50" t="s">
@@ -5432,7 +5443,7 @@
       <c r="C51" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E51" t="s">
@@ -5449,7 +5460,7 @@
       <c r="C52" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="3" t="s">
         <v>168</v>
       </c>
       <c r="E52" t="s">
@@ -5466,7 +5477,7 @@
       <c r="C53" t="s">
         <v>0</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <v>44046</v>
       </c>
       <c r="E53" t="s">
@@ -5483,7 +5494,7 @@
       <c r="C54" t="s">
         <v>212</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="2">
         <v>43985</v>
       </c>
       <c r="E54" t="s">
@@ -5500,7 +5511,7 @@
       <c r="C55" t="s">
         <v>224</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E55" t="s">
@@ -5517,7 +5528,7 @@
       <c r="C56" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E56" t="s">
@@ -5534,7 +5545,7 @@
       <c r="C57" t="s">
         <v>224</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>175</v>
       </c>
       <c r="E57" t="s">
@@ -5551,7 +5562,7 @@
       <c r="C58" t="s">
         <v>224</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E58" t="s">
@@ -5568,7 +5579,7 @@
       <c r="C59" t="s">
         <v>212</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="2">
         <v>43864</v>
       </c>
       <c r="E59" t="s">
@@ -5585,7 +5596,7 @@
       <c r="C60" t="s">
         <v>224</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="3" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5599,7 +5610,7 @@
       <c r="C61" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E61" t="s">
@@ -5616,7 +5627,7 @@
       <c r="C62" t="s">
         <v>212</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="3" t="s">
         <v>168</v>
       </c>
       <c r="E62" t="s">
@@ -5633,7 +5644,7 @@
       <c r="C63" t="s">
         <v>224</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="2">
         <v>43983</v>
       </c>
       <c r="E63" t="s">
@@ -5650,7 +5661,7 @@
       <c r="C64" t="s">
         <v>0</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="2">
         <v>43864</v>
       </c>
       <c r="E64" t="s">
@@ -5667,7 +5678,7 @@
       <c r="C65" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E65" t="s">
@@ -5684,7 +5695,7 @@
       <c r="C66" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="3" t="s">
         <v>168</v>
       </c>
       <c r="E66" t="s">
@@ -5701,7 +5712,7 @@
       <c r="C67" t="s">
         <v>224</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E67" t="s">
@@ -5718,7 +5729,7 @@
       <c r="C68" t="s">
         <v>224</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>189</v>
       </c>
       <c r="E68" t="s">
@@ -5735,7 +5746,7 @@
       <c r="C69" t="s">
         <v>0</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="2">
         <v>44015</v>
       </c>
       <c r="E69" t="s">
@@ -5752,7 +5763,7 @@
       <c r="C70" t="s">
         <v>224</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E70" t="s">
@@ -5769,7 +5780,7 @@
       <c r="C71" t="s">
         <v>5</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E71" t="s">
@@ -5786,7 +5797,7 @@
       <c r="C72" t="s">
         <v>5</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="2">
         <v>43833</v>
       </c>
       <c r="E72" t="s">
@@ -5803,7 +5814,7 @@
       <c r="C73" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="2">
         <v>43954</v>
       </c>
       <c r="E73" t="s">
@@ -5820,7 +5831,7 @@
       <c r="C74" t="s">
         <v>224</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="2">
         <v>43891</v>
       </c>
       <c r="E74" t="s">
@@ -5837,7 +5848,7 @@
       <c r="C75" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E75" t="s">
@@ -5854,7 +5865,7 @@
       <c r="C76" t="s">
         <v>5</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="2">
         <v>43864</v>
       </c>
       <c r="E76" t="s">
@@ -5871,7 +5882,7 @@
       <c r="C77" t="s">
         <v>224</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="3" t="s">
         <v>175</v>
       </c>
       <c r="E77" t="s">
@@ -5888,7 +5899,7 @@
       <c r="C78" t="s">
         <v>224</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="3" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5902,7 +5913,7 @@
       <c r="C79" t="s">
         <v>224</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E79" t="s">
@@ -5919,7 +5930,7 @@
       <c r="C80" t="s">
         <v>224</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="3" t="s">
         <v>203</v>
       </c>
       <c r="E80" t="s">
@@ -5936,7 +5947,7 @@
       <c r="C81" t="s">
         <v>224</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="3" t="s">
         <v>205</v>
       </c>
       <c r="E81" t="s">
@@ -5953,7 +5964,7 @@
       <c r="C82" t="s">
         <v>224</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="3" t="s">
         <v>207</v>
       </c>
       <c r="E82" t="s">
@@ -5970,7 +5981,7 @@
       <c r="C83" t="s">
         <v>224</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="3" t="s">
         <v>177</v>
       </c>
       <c r="E83" t="s">
@@ -5987,7 +5998,7 @@
       <c r="C84" t="s">
         <v>224</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="3" t="s">
         <v>177</v>
       </c>
     </row>
@@ -5999,32 +6010,2450 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F381D50-98E5-477A-8FD8-962A0F786180}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>42.506300000000003</v>
+      </c>
+      <c r="B2">
+        <v>1.5218</v>
+      </c>
+      <c r="C2">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>47.516199999999998</v>
+      </c>
+      <c r="B3">
+        <v>14.5501</v>
+      </c>
+      <c r="C3">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>53.709800000000001</v>
+      </c>
+      <c r="B4">
+        <v>27.953399999999998</v>
+      </c>
+      <c r="C4">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50.833300000000001</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D5">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="2">
+        <v>43923</v>
+      </c>
+      <c r="I5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>43.915900000000001</v>
+      </c>
+      <c r="B6">
+        <v>17.679099999999998</v>
+      </c>
+      <c r="C6">
+        <v>43</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>43954</v>
+      </c>
+      <c r="I6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>45.1</v>
+      </c>
+      <c r="B7">
+        <v>15.2</v>
+      </c>
+      <c r="C7">
+        <v>43</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>49.817500000000003</v>
+      </c>
+      <c r="B8">
+        <v>15.473000000000001</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>43833</v>
+      </c>
+      <c r="I8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>56.2639</v>
+      </c>
+      <c r="B9">
+        <v>9.5017999999999994</v>
+      </c>
+      <c r="C9">
+        <v>43</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>61.892600000000002</v>
+      </c>
+      <c r="B10">
+        <v>-6.9118000000000004</v>
+      </c>
+      <c r="C10">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>211</v>
+      </c>
+      <c r="H10" s="2">
+        <v>43924</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>58.595300000000002</v>
+      </c>
+      <c r="B11">
+        <v>25.0136</v>
+      </c>
+      <c r="C11">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D12">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" t="s">
+        <v>224</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D13">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s">
+        <v>224</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D14">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>39.074199999999998</v>
+      </c>
+      <c r="B15">
+        <v>21.824300000000001</v>
+      </c>
+      <c r="C15">
+        <v>43</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>47.162500000000001</v>
+      </c>
+      <c r="B16">
+        <v>19.503299999999999</v>
+      </c>
+      <c r="C16">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>43924</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>64.963099999999997</v>
+      </c>
+      <c r="B17">
+        <v>-19.020800000000001</v>
+      </c>
+      <c r="C17">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>53.142400000000002</v>
+      </c>
+      <c r="B18">
+        <v>-7.6920999999999999</v>
+      </c>
+      <c r="C18">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D19">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" t="s">
+        <v>224</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>56.879600000000003</v>
+      </c>
+      <c r="B20">
+        <v>24.603200000000001</v>
+      </c>
+      <c r="C20">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>47.14</v>
+      </c>
+      <c r="B21">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="C21">
+        <v>46.818199999999997</v>
+      </c>
+      <c r="D21">
+        <v>8.2274999999999991</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" t="s">
+        <v>211</v>
+      </c>
+      <c r="H21" s="2">
+        <v>43893</v>
+      </c>
+      <c r="I21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>55.169400000000003</v>
+      </c>
+      <c r="B22">
+        <v>23.8813</v>
+      </c>
+      <c r="C22">
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>49.815300000000001</v>
+      </c>
+      <c r="B23">
+        <v>6.1295999999999999</v>
+      </c>
+      <c r="C23">
+        <v>43</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>43.7333</v>
+      </c>
+      <c r="B24">
+        <v>7.4166999999999996</v>
+      </c>
+      <c r="C24" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D24">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" t="s">
+        <v>224</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>52.132599999999996</v>
+      </c>
+      <c r="B25">
+        <v>5.2912999999999997</v>
+      </c>
+      <c r="C25">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>41.608600000000003</v>
+      </c>
+      <c r="B26">
+        <v>21.7453</v>
+      </c>
+      <c r="C26">
+        <v>43</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>60.472000000000001</v>
+      </c>
+      <c r="B27">
+        <v>8.4688999999999997</v>
+      </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>51.919400000000003</v>
+      </c>
+      <c r="B28">
+        <v>19.145099999999999</v>
+      </c>
+      <c r="C28">
+        <v>51</v>
+      </c>
+      <c r="D28">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>211</v>
+      </c>
+      <c r="H28" s="2">
+        <v>43924</v>
+      </c>
+      <c r="I28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>39.399900000000002</v>
+      </c>
+      <c r="B29">
+        <v>-8.2245000000000008</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>-4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" t="s">
+        <v>211</v>
+      </c>
+      <c r="H29" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>45.943199999999997</v>
+      </c>
+      <c r="B30">
+        <v>24.966799999999999</v>
+      </c>
+      <c r="C30">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>60</v>
+      </c>
+      <c r="B31">
+        <v>90</v>
+      </c>
+      <c r="C31">
+        <v>43</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>43.942399999999999</v>
+      </c>
+      <c r="B32">
+        <v>12.457800000000001</v>
+      </c>
+      <c r="C32">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>46.151200000000003</v>
+      </c>
+      <c r="B33">
+        <v>14.9955</v>
+      </c>
+      <c r="C33">
+        <v>43</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>43954</v>
+      </c>
+      <c r="I33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>40</v>
+      </c>
+      <c r="B34">
+        <v>-4</v>
+      </c>
+      <c r="C34">
+        <v>51</v>
+      </c>
+      <c r="D34">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" t="s">
+        <v>211</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>63</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D35">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" t="s">
+        <v>224</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>46.818199999999997</v>
+      </c>
+      <c r="B36">
+        <v>8.2274999999999991</v>
+      </c>
+      <c r="C36">
+        <v>43</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>48.379399999999997</v>
+      </c>
+      <c r="B37">
+        <v>31.165600000000001</v>
+      </c>
+      <c r="C37">
+        <v>43</v>
+      </c>
+      <c r="D37">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>63</v>
+      </c>
+      <c r="F37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>43954</v>
+      </c>
+      <c r="I37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>55</v>
+      </c>
+      <c r="B38">
+        <v>-3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D38">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E38" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" t="s">
+        <v>224</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36.140799999999999</v>
+      </c>
+      <c r="B39">
+        <v>-5.3536000000000001</v>
+      </c>
+      <c r="C39">
+        <v>43</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>43926</v>
+      </c>
+      <c r="I39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>28.033899999999999</v>
+      </c>
+      <c r="B40">
+        <v>1.6596</v>
+      </c>
+      <c r="C40">
+        <v>47</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
+        <v>211</v>
+      </c>
+      <c r="H40" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3.8479999999999999</v>
+      </c>
+      <c r="B41">
+        <v>11.5021</v>
+      </c>
+      <c r="C41">
+        <v>47</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s">
+        <v>211</v>
+      </c>
+      <c r="H41" s="2">
+        <v>43985</v>
+      </c>
+      <c r="I41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>26</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D42">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" t="s">
+        <v>224</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>31.791699999999999</v>
+      </c>
+      <c r="B43">
+        <v>-7.0926</v>
+      </c>
+      <c r="C43">
+        <v>43</v>
+      </c>
+      <c r="D43">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>133</v>
+      </c>
+      <c r="F43" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>9.0820000000000007</v>
+      </c>
+      <c r="B44">
+        <v>8.6753</v>
+      </c>
+      <c r="C44">
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F44" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>14.497400000000001</v>
+      </c>
+      <c r="B45">
+        <v>-14.452400000000001</v>
+      </c>
+      <c r="C45">
+        <v>47</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
+        <v>211</v>
+      </c>
+      <c r="H45" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>-30.5595</v>
+      </c>
+      <c r="B46">
+        <v>22.9375</v>
+      </c>
+      <c r="C46">
+        <v>43</v>
+      </c>
+      <c r="D46">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>43954</v>
+      </c>
+      <c r="I46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>8.6195000000000004</v>
+      </c>
+      <c r="B47">
+        <v>0.82479999999999998</v>
+      </c>
+      <c r="C47">
+        <v>51</v>
+      </c>
+      <c r="D47">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>150</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>211</v>
+      </c>
+      <c r="H47" s="2">
+        <v>43985</v>
+      </c>
+      <c r="I47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>34</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>43</v>
+      </c>
+      <c r="D48">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s">
+        <v>140</v>
+      </c>
+      <c r="F48" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>33</v>
+      </c>
+      <c r="B49">
+        <v>65</v>
+      </c>
+      <c r="C49">
+        <v>32</v>
+      </c>
+      <c r="D49">
+        <v>53</v>
+      </c>
+      <c r="E49" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>40.069099999999999</v>
+      </c>
+      <c r="B50">
+        <v>45.038200000000003</v>
+      </c>
+      <c r="C50">
+        <v>32</v>
+      </c>
+      <c r="D50">
+        <v>53</v>
+      </c>
+      <c r="E50" t="s">
+        <v>130</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>40.143099999999997</v>
+      </c>
+      <c r="B51">
+        <v>47.576900000000002</v>
+      </c>
+      <c r="C51">
+        <v>32</v>
+      </c>
+      <c r="D51">
+        <v>53</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I51" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>26.0275</v>
+      </c>
+      <c r="B52">
+        <v>50.55</v>
+      </c>
+      <c r="C52">
+        <v>32</v>
+      </c>
+      <c r="D52">
+        <v>53</v>
+      </c>
+      <c r="E52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>33.854700000000001</v>
+      </c>
+      <c r="B53">
+        <v>35.862299999999998</v>
+      </c>
+      <c r="C53">
+        <v>43</v>
+      </c>
+      <c r="D53">
+        <v>12</v>
+      </c>
+      <c r="E53" t="s">
+        <v>170</v>
+      </c>
+      <c r="F53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2">
+        <v>44046</v>
+      </c>
+      <c r="I53" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>27.514199999999999</v>
+      </c>
+      <c r="B54">
+        <v>90.433599999999998</v>
+      </c>
+      <c r="C54">
+        <v>21</v>
+      </c>
+      <c r="D54">
+        <v>78</v>
+      </c>
+      <c r="E54" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" t="s">
+        <v>110</v>
+      </c>
+      <c r="G54" t="s">
+        <v>212</v>
+      </c>
+      <c r="H54" s="2">
+        <v>43985</v>
+      </c>
+      <c r="I54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>11.55</v>
+      </c>
+      <c r="B55">
+        <v>104.91670000000001</v>
+      </c>
+      <c r="C55" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D55">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E55" t="s">
+        <v>106</v>
+      </c>
+      <c r="F55" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" t="s">
+        <v>224</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>42.315399999999997</v>
+      </c>
+      <c r="B56">
+        <v>43.356900000000003</v>
+      </c>
+      <c r="C56">
+        <v>32</v>
+      </c>
+      <c r="D56">
+        <v>53</v>
+      </c>
+      <c r="E56" t="s">
+        <v>152</v>
+      </c>
+      <c r="F56" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" t="s">
+        <v>5</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>22.3</v>
+      </c>
+      <c r="B57">
+        <v>114.2</v>
+      </c>
+      <c r="C57" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D57">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E57" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" t="s">
+        <v>224</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I57" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>21</v>
+      </c>
+      <c r="B58">
+        <v>78</v>
+      </c>
+      <c r="C58" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D58">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E58" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" t="s">
+        <v>92</v>
+      </c>
+      <c r="G58" t="s">
+        <v>224</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>-0.7893</v>
+      </c>
+      <c r="B59">
+        <v>113.9213</v>
+      </c>
+      <c r="C59">
+        <v>36</v>
+      </c>
+      <c r="D59">
+        <v>138</v>
+      </c>
+      <c r="E59" t="s">
+        <v>132</v>
+      </c>
+      <c r="F59" t="s">
+        <v>94</v>
+      </c>
+      <c r="G59" t="s">
+        <v>212</v>
+      </c>
+      <c r="H59" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I59" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>32</v>
+      </c>
+      <c r="B60">
+        <v>53</v>
+      </c>
+      <c r="C60" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D60">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" t="s">
+        <v>224</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>33</v>
+      </c>
+      <c r="B61">
+        <v>44</v>
+      </c>
+      <c r="C61">
+        <v>32</v>
+      </c>
+      <c r="D61">
+        <v>53</v>
+      </c>
+      <c r="E61" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I61" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>31</v>
+      </c>
+      <c r="B62">
+        <v>35</v>
+      </c>
+      <c r="C62">
+        <v>36</v>
+      </c>
+      <c r="D62">
+        <v>138</v>
+      </c>
+      <c r="E62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" t="s">
+        <v>94</v>
+      </c>
+      <c r="G62" t="s">
+        <v>212</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I62" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>36</v>
+      </c>
+      <c r="B63">
+        <v>138</v>
+      </c>
+      <c r="C63" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D63">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E63" t="s">
+        <v>94</v>
+      </c>
+      <c r="F63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G63" t="s">
+        <v>224</v>
+      </c>
+      <c r="H63" s="2">
+        <v>43983</v>
+      </c>
+      <c r="I63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>31.24</v>
+      </c>
+      <c r="B64">
+        <v>36.51</v>
+      </c>
+      <c r="C64">
+        <v>43</v>
+      </c>
+      <c r="D64">
+        <v>12</v>
+      </c>
+      <c r="E64" t="s">
+        <v>138</v>
+      </c>
+      <c r="F64" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" t="s">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I64" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>29.5</v>
+      </c>
+      <c r="B65">
+        <v>47.75</v>
+      </c>
+      <c r="C65">
+        <v>32</v>
+      </c>
+      <c r="D65">
+        <v>53</v>
+      </c>
+      <c r="E65" t="s">
+        <v>119</v>
+      </c>
+      <c r="F65" t="s">
+        <v>5</v>
+      </c>
+      <c r="G65" t="s">
+        <v>5</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I65" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>33.888629999999999</v>
+      </c>
+      <c r="B66">
+        <v>35.495480000000001</v>
+      </c>
+      <c r="C66">
+        <v>32</v>
+      </c>
+      <c r="D66">
+        <v>53</v>
+      </c>
+      <c r="E66" t="s">
+        <v>114</v>
+      </c>
+      <c r="F66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" t="s">
+        <v>5</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I66" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>22.166699999999999</v>
+      </c>
+      <c r="B67">
+        <v>113.55</v>
+      </c>
+      <c r="C67" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D67">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E67" t="s">
+        <v>98</v>
+      </c>
+      <c r="F67" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" t="s">
+        <v>224</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I67" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2.5</v>
+      </c>
+      <c r="B68">
+        <v>112.5</v>
+      </c>
+      <c r="C68" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D68">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E68" t="s">
+        <v>103</v>
+      </c>
+      <c r="F68" t="s">
+        <v>92</v>
+      </c>
+      <c r="G68" t="s">
+        <v>224</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I68" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>3.2027999999999999</v>
+      </c>
+      <c r="B69">
+        <v>73.220699999999994</v>
+      </c>
+      <c r="C69">
+        <v>43</v>
+      </c>
+      <c r="D69">
+        <v>12</v>
+      </c>
+      <c r="E69" t="s">
+        <v>191</v>
+      </c>
+      <c r="F69" t="s">
+        <v>0</v>
+      </c>
+      <c r="G69" t="s">
+        <v>0</v>
+      </c>
+      <c r="H69" s="2">
+        <v>44015</v>
+      </c>
+      <c r="I69" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>28.166699999999999</v>
+      </c>
+      <c r="B70">
+        <v>84.25</v>
+      </c>
+      <c r="C70" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D70">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E70" t="s">
+        <v>102</v>
+      </c>
+      <c r="F70" t="s">
+        <v>92</v>
+      </c>
+      <c r="G70" t="s">
+        <v>224</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I70" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>21</v>
+      </c>
+      <c r="B71">
+        <v>57</v>
+      </c>
+      <c r="C71">
+        <v>32</v>
+      </c>
+      <c r="D71">
+        <v>53</v>
+      </c>
+      <c r="E71" t="s">
+        <v>116</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" t="s">
+        <v>5</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I71" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>30.375299999999999</v>
+      </c>
+      <c r="B72">
+        <v>69.345100000000002</v>
+      </c>
+      <c r="C72">
+        <v>32</v>
+      </c>
+      <c r="D72">
+        <v>53</v>
+      </c>
+      <c r="E72" t="s">
+        <v>122</v>
+      </c>
+      <c r="F72" t="s">
+        <v>5</v>
+      </c>
+      <c r="G72" t="s">
+        <v>5</v>
+      </c>
+      <c r="H72" s="2">
+        <v>43833</v>
+      </c>
+      <c r="I72" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>31.952200000000001</v>
+      </c>
+      <c r="B73">
+        <v>35.233199999999997</v>
+      </c>
+      <c r="C73">
+        <v>32</v>
+      </c>
+      <c r="D73">
+        <v>53</v>
+      </c>
+      <c r="E73" t="s">
+        <v>141</v>
+      </c>
+      <c r="F73" t="s">
+        <v>5</v>
+      </c>
+      <c r="G73" t="s">
+        <v>5</v>
+      </c>
+      <c r="H73" s="2">
+        <v>43954</v>
+      </c>
+      <c r="I73" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74">
+        <v>122</v>
+      </c>
+      <c r="C74" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D74">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E74" t="s">
+        <v>109</v>
+      </c>
+      <c r="F74" t="s">
+        <v>92</v>
+      </c>
+      <c r="G74" t="s">
+        <v>224</v>
+      </c>
+      <c r="H74" s="2">
+        <v>43891</v>
+      </c>
+      <c r="I74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>25.354800000000001</v>
+      </c>
+      <c r="B75">
+        <v>51.183900000000001</v>
+      </c>
+      <c r="C75">
+        <v>32</v>
+      </c>
+      <c r="D75">
+        <v>53</v>
+      </c>
+      <c r="E75" t="s">
+        <v>128</v>
+      </c>
+      <c r="F75" t="s">
+        <v>5</v>
+      </c>
+      <c r="G75" t="s">
+        <v>5</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I75" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>24</v>
+      </c>
+      <c r="B76">
+        <v>45</v>
+      </c>
+      <c r="C76">
+        <v>32</v>
+      </c>
+      <c r="D76">
+        <v>53</v>
+      </c>
+      <c r="E76" t="s">
+        <v>134</v>
+      </c>
+      <c r="F76" t="s">
+        <v>5</v>
+      </c>
+      <c r="G76" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="2">
+        <v>43864</v>
+      </c>
+      <c r="I76" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1.2833000000000001</v>
+      </c>
+      <c r="B77">
+        <v>103.83329999999999</v>
+      </c>
+      <c r="C77" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D77">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E77" t="s">
+        <v>100</v>
+      </c>
+      <c r="F77" t="s">
+        <v>92</v>
+      </c>
+      <c r="G77" t="s">
+        <v>224</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I77" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>36</v>
+      </c>
+      <c r="B78">
+        <v>128</v>
+      </c>
+      <c r="C78" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D78">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E78" t="s">
+        <v>95</v>
+      </c>
+      <c r="F78" t="s">
+        <v>92</v>
+      </c>
+      <c r="G78" t="s">
+        <v>224</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>7</v>
+      </c>
+      <c r="B79">
+        <v>81</v>
+      </c>
+      <c r="C79" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D79">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E79" t="s">
+        <v>107</v>
+      </c>
+      <c r="F79" t="s">
+        <v>92</v>
+      </c>
+      <c r="G79" t="s">
+        <v>224</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I79" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>23.7</v>
+      </c>
+      <c r="B80">
+        <v>121</v>
+      </c>
+      <c r="C80" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D80">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E80" t="s">
+        <v>96</v>
+      </c>
+      <c r="F80" t="s">
+        <v>92</v>
+      </c>
+      <c r="G80" t="s">
+        <v>224</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I80" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <v>101</v>
+      </c>
+      <c r="C81" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D81">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E81" t="s">
+        <v>93</v>
+      </c>
+      <c r="F81" t="s">
+        <v>92</v>
+      </c>
+      <c r="G81" t="s">
+        <v>224</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I81" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>24</v>
+      </c>
+      <c r="B82">
+        <v>54</v>
+      </c>
+      <c r="C82" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D82">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E82" t="s">
+        <v>108</v>
+      </c>
+      <c r="F82" t="s">
+        <v>92</v>
+      </c>
+      <c r="G82" t="s">
+        <v>224</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="I82" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>16</v>
+      </c>
+      <c r="B83">
+        <v>108</v>
+      </c>
+      <c r="C83" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D83">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E83" t="s">
+        <v>101</v>
+      </c>
+      <c r="F83" t="s">
+        <v>92</v>
+      </c>
+      <c r="G83" t="s">
+        <v>224</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I83" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>38.764600000000002</v>
+      </c>
+      <c r="B84">
+        <v>-95</v>
+      </c>
+      <c r="C84" s="1">
+        <v>30.9756</v>
+      </c>
+      <c r="D84">
+        <v>104.27070000000001</v>
+      </c>
+      <c r="E84" t="s">
+        <v>97</v>
+      </c>
+      <c r="F84" t="s">
+        <v>92</v>
+      </c>
+      <c r="G84" t="s">
+        <v>224</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated data and origin map
</commit_message>
<xml_diff>
--- a/data/coronavirus_origin_data.xlsx
+++ b/data/coronavirus_origin_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\OneDrive\FYP2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE50AB3B-EDE1-4DBA-BF26-3CDF13AC78DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC42140-ACAC-4DDF-A72B-A35E1065D571}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="1000" activeTab="5" xr2:uid="{BBD3DD9A-9B31-49E4-9DF5-3A64C89D46D5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="296">
   <si>
     <t>Italy</t>
   </si>
@@ -786,6 +786,144 @@
   </si>
   <si>
     <t>origin_long</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>The patient is a 33-year-old man in the city of Talca</t>
+  </si>
+  <si>
+    <t>A 19-year-old female patient who recently travelled to Milan, Italy</t>
+  </si>
+  <si>
+    <t>The patient, a woman in her 70s, Ecuadorian citizen which resides in Spain, had arrived to Guayaquil on 14 February</t>
+  </si>
+  <si>
+    <t>Health Minister Aníbal Cruz confirmed the first two cases on March 10. Both involved women in their 60s who had traveled to Italy. One woman in the city of Oruro was isolated in her home while the other in the Santa Cruz department was quarantined in a health facility.</t>
+  </si>
+  <si>
+    <t>China is Argentina’s second-biggest export destination and the outbreak is already hitting trade. A 43 year old man had travelled around in Europe both visiting Hungary and Spain, and departed from Italy, Milan, on 1st of March.</t>
+  </si>
+  <si>
+    <t>Brazil confirmed Latin America’s first case on February 26: a 61-year-old man who had recently returned to São Paulo from a business trip to northern Italy.</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Official Cuban broadcast media confirmed the island’s first three cases on March 11. The three Italian tourists traveled to Havana on March 9 and have been quarantined at the Pedro Kourí Tropical Medicine Institute in the capital</t>
+  </si>
+  <si>
+    <t>On March 6, Costa Rica became the first Central American country to confirm a case, involving a 49-year-old tourist visiting from the United States</t>
+  </si>
+  <si>
+    <t>The DR’s first confirmed case was reported on March 1. The 62-year-old Italian tourist was quarantined in a military hospital in San Isidro, near Santo Domingo. </t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>The country’s first cases involve two women who traveled to Europe: a 42-year-old who arrived from Spain and a 37-year-old who returned from Switzerland</t>
+  </si>
+  <si>
+    <t>The country confirmed its first case, involving a 35-year-old man in Mexico City who was placed in quarantine, on February 28. The first three people confirmed to be carriers all caught the virus during a February conference in Bergamo, Italy, while the subsequent two cases involved students who had studied in Milan. </t>
+  </si>
+  <si>
+    <t>A 40-year-old Panamanian woman who had traveled to Spain became the country’s first confirmed case of coronavirus, Panama’s Ministry of Health and President Laurentino Cortizo announced on March 9.</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Paraguay's Health Ministry confirmed the country's first case on March 7 via Twitter. The 32-year-old man, who was quarantined in his home, had traveled to Ecuador for business.</t>
+  </si>
+  <si>
+    <t>Peru confirmed its first case on March 6. The 25-year-old man had recently returned from a trip that took him to Spain, France, and the Czech Republic</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>A female patient who arrived from the United Kingdom on 4 March 2020. The health minister reported that she has been in isolation since 9 March 2020 after showing respiratory symptoms. Following the update, the travel ban imposed was expanded to include France, Germany and Spain</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Matinique</t>
+  </si>
+  <si>
+    <t>Health Minister Claudine Lougue told reporters that the two patients, a husband and wife, had recently returned to Burkina Faso from a trip to France and were now in isolation.</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>The patient is a Belgian citizen who had been in Congo for several days</t>
+  </si>
+  <si>
+    <t>Estwatini</t>
+  </si>
+  <si>
+    <t>03/14/2020</t>
+  </si>
+  <si>
+    <t>A 33-year-old woman, who returned from the United States at the end of February and then travelled to Lesotho before returning home to Eswatini, is currently in isolation</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>03/13/2020</t>
+  </si>
+  <si>
+    <t>On 13 March 2020, the first coronavirus case was reported in the county and the victim later identified was a Japanese citizen</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>The country's first case was announced on 12 March, a 27 year old Gabonese man who returned to Gabon from France, 4 days prior to confirmation of the coronavirus</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Ghana reported it's first two cases on 12 March. The two cases were people who came back to the country from Norway and Turkey, with the contract tracing process beginning</t>
+  </si>
+  <si>
+    <t>An employee of the European Union delegation in Guinea has tested positive for coronavirus, a delegation spokesman said on Friday, in Guinea's first confirmed case of the virus</t>
+  </si>
+  <si>
+    <t>Ivory Coast</t>
+  </si>
+  <si>
+    <t>The Ivory Coast has confirmed its first case of the coronavirus in a 45-year-old citizen who had recently returned from Italy, the country's health ministry said Wednesday.</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>On 13 March, the first case in Kenya was confirmed, a woman who came from the US via London.</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>A statement from the health ministry, also released on Friday, said the man was an "expatriate" who had flown into Mauritania from Europe on Monday.</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Namibia said a couple visiting from Spain tested positive for the coronavirus, the first cases of the disease in the southwest African nation.</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Rwanda has confirmed its first case of coronavirus, an Indian citizen who arrived in the East African nation from Mumbai on March 8, the Health Ministry said on Saturday</t>
   </si>
 </sst>
 </file>
@@ -827,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -839,6 +977,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3973,7 +4112,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4571,9 +4710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D086343C-F872-446A-BD7D-B96E4ED95CA5}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection sqref="A1:E84"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6010,10 +6147,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F381D50-98E5-477A-8FD8-962A0F786180}">
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6023,6 +6160,7 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7150,7 +7288,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="2">
-        <v>43926</v>
+        <v>43954</v>
       </c>
       <c r="I39" t="s">
         <v>67</v>
@@ -7236,7 +7374,7 @@
       <c r="G42" t="s">
         <v>224</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="2" t="s">
         <v>213</v>
       </c>
       <c r="I42" t="s">
@@ -7294,7 +7432,7 @@
       <c r="G44" t="s">
         <v>0</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="2" t="s">
         <v>83</v>
       </c>
       <c r="I44" t="s">
@@ -7439,7 +7577,7 @@
       <c r="G49" t="s">
         <v>5</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I49" t="s">
@@ -7468,7 +7606,7 @@
       <c r="G50" t="s">
         <v>5</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I50" t="s">
@@ -7497,7 +7635,7 @@
       <c r="G51" t="s">
         <v>5</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="H51" s="2" t="s">
         <v>82</v>
       </c>
       <c r="I51" t="s">
@@ -7526,7 +7664,7 @@
       <c r="G52" t="s">
         <v>5</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" s="2" t="s">
         <v>168</v>
       </c>
       <c r="I52" t="s">
@@ -7613,7 +7751,7 @@
       <c r="G55" t="s">
         <v>224</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" s="2" t="s">
         <v>86</v>
       </c>
       <c r="I55" t="s">
@@ -7642,7 +7780,7 @@
       <c r="G56" t="s">
         <v>5</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H56" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I56" t="s">
@@ -7671,7 +7809,7 @@
       <c r="G57" t="s">
         <v>224</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H57" s="2" t="s">
         <v>175</v>
       </c>
       <c r="I57" t="s">
@@ -7700,7 +7838,7 @@
       <c r="G58" t="s">
         <v>224</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H58" s="2" t="s">
         <v>179</v>
       </c>
       <c r="I58" t="s">
@@ -7758,7 +7896,7 @@
       <c r="G60" t="s">
         <v>224</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H60" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -7784,7 +7922,7 @@
       <c r="G61" t="s">
         <v>5</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H61" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I61" t="s">
@@ -7813,7 +7951,7 @@
       <c r="G62" t="s">
         <v>212</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="2" t="s">
         <v>168</v>
       </c>
       <c r="I62" t="s">
@@ -7900,7 +8038,7 @@
       <c r="G65" t="s">
         <v>5</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I65" t="s">
@@ -7929,7 +8067,7 @@
       <c r="G66" t="s">
         <v>5</v>
       </c>
-      <c r="H66" s="3" t="s">
+      <c r="H66" s="2" t="s">
         <v>168</v>
       </c>
       <c r="I66" t="s">
@@ -7958,7 +8096,7 @@
       <c r="G67" t="s">
         <v>224</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H67" s="2" t="s">
         <v>177</v>
       </c>
       <c r="I67" t="s">
@@ -7987,7 +8125,7 @@
       <c r="G68" t="s">
         <v>224</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="2" t="s">
         <v>189</v>
       </c>
       <c r="I68" t="s">
@@ -8045,7 +8183,7 @@
       <c r="G70" t="s">
         <v>224</v>
       </c>
-      <c r="H70" s="3" t="s">
+      <c r="H70" s="2" t="s">
         <v>85</v>
       </c>
       <c r="I70" t="s">
@@ -8074,7 +8212,7 @@
       <c r="G71" t="s">
         <v>5</v>
       </c>
-      <c r="H71" s="3" t="s">
+      <c r="H71" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I71" t="s">
@@ -8190,7 +8328,7 @@
       <c r="G75" t="s">
         <v>5</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="H75" s="2" t="s">
         <v>83</v>
       </c>
       <c r="I75" t="s">
@@ -8248,7 +8386,7 @@
       <c r="G77" t="s">
         <v>224</v>
       </c>
-      <c r="H77" s="3" t="s">
+      <c r="H77" s="2" t="s">
         <v>175</v>
       </c>
       <c r="I77" t="s">
@@ -8277,7 +8415,7 @@
       <c r="G78" t="s">
         <v>224</v>
       </c>
-      <c r="H78" s="3" t="s">
+      <c r="H78" s="2" t="s">
         <v>201</v>
       </c>
     </row>
@@ -8303,7 +8441,7 @@
       <c r="G79" t="s">
         <v>224</v>
       </c>
-      <c r="H79" s="3" t="s">
+      <c r="H79" s="2" t="s">
         <v>86</v>
       </c>
       <c r="I79" t="s">
@@ -8332,7 +8470,7 @@
       <c r="G80" t="s">
         <v>224</v>
       </c>
-      <c r="H80" s="3" t="s">
+      <c r="H80" s="2" t="s">
         <v>203</v>
       </c>
       <c r="I80" t="s">
@@ -8361,7 +8499,7 @@
       <c r="G81" t="s">
         <v>224</v>
       </c>
-      <c r="H81" s="3" t="s">
+      <c r="H81" s="2" t="s">
         <v>205</v>
       </c>
       <c r="I81" t="s">
@@ -8390,7 +8528,7 @@
       <c r="G82" t="s">
         <v>224</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H82" s="2" t="s">
         <v>207</v>
       </c>
       <c r="I82" t="s">
@@ -8419,7 +8557,7 @@
       <c r="G83" t="s">
         <v>224</v>
       </c>
-      <c r="H83" s="3" t="s">
+      <c r="H83" s="2" t="s">
         <v>177</v>
       </c>
       <c r="I83" t="s">
@@ -8448,8 +8586,869 @@
       <c r="G84" t="s">
         <v>224</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H84" s="2" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>-38.416097000000001</v>
+      </c>
+      <c r="B85">
+        <v>-63.616672000000001</v>
+      </c>
+      <c r="C85">
+        <v>43</v>
+      </c>
+      <c r="D85">
+        <v>12</v>
+      </c>
+      <c r="E85" t="s">
+        <v>136</v>
+      </c>
+      <c r="F85" t="s">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s">
+        <v>0</v>
+      </c>
+      <c r="H85" s="7">
+        <v>43893</v>
+      </c>
+      <c r="I85" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>-16.290154000000001</v>
+      </c>
+      <c r="B86">
+        <v>-63.588653000000001</v>
+      </c>
+      <c r="C86">
+        <v>43</v>
+      </c>
+      <c r="D86">
+        <v>12</v>
+      </c>
+      <c r="E86" t="s">
+        <v>250</v>
+      </c>
+      <c r="F86" t="s">
+        <v>0</v>
+      </c>
+      <c r="G86" t="s">
+        <v>0</v>
+      </c>
+      <c r="H86" s="7">
+        <v>44107</v>
+      </c>
+      <c r="I86" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>-14.235004</v>
+      </c>
+      <c r="B87">
+        <v>-51.925280000000001</v>
+      </c>
+      <c r="C87">
+        <v>43</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>123</v>
+      </c>
+      <c r="F87" t="s">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>0</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I87" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>-35.675147000000003</v>
+      </c>
+      <c r="B88">
+        <v>-71.542968999999999</v>
+      </c>
+      <c r="C88">
+        <v>43</v>
+      </c>
+      <c r="D88">
+        <v>12</v>
+      </c>
+      <c r="E88" t="s">
+        <v>137</v>
+      </c>
+      <c r="F88" t="s">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
+        <v>0</v>
+      </c>
+      <c r="H88" s="7">
+        <v>43893</v>
+      </c>
+      <c r="I88" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>4.5708679999999999</v>
+      </c>
+      <c r="B89">
+        <v>-74.297332999999995</v>
+      </c>
+      <c r="C89">
+        <v>43</v>
+      </c>
+      <c r="D89">
+        <v>12</v>
+      </c>
+      <c r="E89" t="s">
+        <v>145</v>
+      </c>
+      <c r="F89" t="s">
+        <v>0</v>
+      </c>
+      <c r="G89" t="s">
+        <v>0</v>
+      </c>
+      <c r="H89" s="7">
+        <v>43985</v>
+      </c>
+      <c r="I89" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>21.521757000000001</v>
+      </c>
+      <c r="B90">
+        <v>-77.781166999999996</v>
+      </c>
+      <c r="C90">
+        <v>43</v>
+      </c>
+      <c r="D90">
+        <v>12</v>
+      </c>
+      <c r="E90" t="s">
+        <v>257</v>
+      </c>
+      <c r="F90" t="s">
+        <v>0</v>
+      </c>
+      <c r="G90" t="s">
+        <v>0</v>
+      </c>
+      <c r="H90" s="7">
+        <v>44138</v>
+      </c>
+      <c r="I90" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>9.7489170000000005</v>
+      </c>
+      <c r="B91">
+        <v>-83.753428</v>
+      </c>
+      <c r="C91">
+        <v>38.764600000000002</v>
+      </c>
+      <c r="D91">
+        <v>-95</v>
+      </c>
+      <c r="E91" t="s">
+        <v>146</v>
+      </c>
+      <c r="F91" t="s">
+        <v>97</v>
+      </c>
+      <c r="G91" t="s">
+        <v>265</v>
+      </c>
+      <c r="H91" s="7">
+        <v>43985</v>
+      </c>
+      <c r="I91" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>18.735693000000001</v>
+      </c>
+      <c r="B92">
+        <v>-70.162650999999997</v>
+      </c>
+      <c r="C92">
+        <v>43</v>
+      </c>
+      <c r="D92">
+        <v>12</v>
+      </c>
+      <c r="E92" t="s">
+        <v>131</v>
+      </c>
+      <c r="F92" t="s">
+        <v>0</v>
+      </c>
+      <c r="G92" t="s">
+        <v>0</v>
+      </c>
+      <c r="H92" s="7">
+        <v>43833</v>
+      </c>
+      <c r="I92" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>-1.8312390000000001</v>
+      </c>
+      <c r="B93">
+        <v>-78.183406000000005</v>
+      </c>
+      <c r="C93">
+        <v>40</v>
+      </c>
+      <c r="D93">
+        <v>-4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>129</v>
+      </c>
+      <c r="F93" t="s">
+        <v>48</v>
+      </c>
+      <c r="G93" t="s">
+        <v>211</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I93" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>3.9338890000000002</v>
+      </c>
+      <c r="B94">
+        <v>-53.125782000000001</v>
+      </c>
+      <c r="C94">
+        <v>38.764600000000002</v>
+      </c>
+      <c r="D94">
+        <v>-95</v>
+      </c>
+      <c r="E94" t="s">
+        <v>235</v>
+      </c>
+      <c r="F94" t="s">
+        <v>97</v>
+      </c>
+      <c r="G94" t="s">
+        <v>265</v>
+      </c>
+      <c r="H94" s="7">
+        <v>43985</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>15.199999</v>
+      </c>
+      <c r="B95">
+        <v>-86.241905000000003</v>
+      </c>
+      <c r="C95">
+        <v>40</v>
+      </c>
+      <c r="D95">
+        <v>-4</v>
+      </c>
+      <c r="E95" t="s">
+        <v>261</v>
+      </c>
+      <c r="F95" t="s">
+        <v>48</v>
+      </c>
+      <c r="G95" t="s">
+        <v>211</v>
+      </c>
+      <c r="H95" s="7">
+        <v>44138</v>
+      </c>
+      <c r="I95" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>23.634501</v>
+      </c>
+      <c r="B96">
+        <v>-102.552784</v>
+      </c>
+      <c r="C96">
+        <v>43</v>
+      </c>
+      <c r="D96">
+        <v>12</v>
+      </c>
+      <c r="E96" t="s">
+        <v>124</v>
+      </c>
+      <c r="F96" t="s">
+        <v>0</v>
+      </c>
+      <c r="G96" t="s">
+        <v>0</v>
+      </c>
+      <c r="H96" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I96" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>8.5379810000000003</v>
+      </c>
+      <c r="B97">
+        <v>-80.782127000000003</v>
+      </c>
+      <c r="C97">
+        <v>40</v>
+      </c>
+      <c r="D97">
+        <v>-4</v>
+      </c>
+      <c r="E97" t="s">
+        <v>232</v>
+      </c>
+      <c r="F97" t="s">
+        <v>48</v>
+      </c>
+      <c r="G97" t="s">
+        <v>211</v>
+      </c>
+      <c r="H97" s="7">
+        <v>44077</v>
+      </c>
+      <c r="I97" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>-23.442502999999999</v>
+      </c>
+      <c r="B98">
+        <v>-58.443832</v>
+      </c>
+      <c r="C98">
+        <v>-1.8312390000000001</v>
+      </c>
+      <c r="D98">
+        <v>-78.183406000000005</v>
+      </c>
+      <c r="E98" t="s">
+        <v>239</v>
+      </c>
+      <c r="F98" t="s">
+        <v>129</v>
+      </c>
+      <c r="G98" t="s">
+        <v>265</v>
+      </c>
+      <c r="H98" s="7">
+        <v>44015</v>
+      </c>
+      <c r="I98" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>-9.1899669999999993</v>
+      </c>
+      <c r="B99">
+        <v>-75.015152</v>
+      </c>
+      <c r="C99">
+        <v>47</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>147</v>
+      </c>
+      <c r="F99" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" t="s">
+        <v>211</v>
+      </c>
+      <c r="H99" s="7">
+        <v>43985</v>
+      </c>
+      <c r="I99" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>18.109580999999999</v>
+      </c>
+      <c r="B100">
+        <v>-77.297507999999993</v>
+      </c>
+      <c r="C100">
+        <v>55</v>
+      </c>
+      <c r="D100">
+        <v>-3</v>
+      </c>
+      <c r="E100" t="s">
+        <v>268</v>
+      </c>
+      <c r="F100" t="s">
+        <v>111</v>
+      </c>
+      <c r="G100" t="s">
+        <v>211</v>
+      </c>
+      <c r="H100" s="7">
+        <v>44107</v>
+      </c>
+      <c r="I100" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>4.8604159999999998</v>
+      </c>
+      <c r="B101">
+        <v>-58.93018</v>
+      </c>
+      <c r="C101">
+        <v>38.764600000000002</v>
+      </c>
+      <c r="D101">
+        <v>-95</v>
+      </c>
+      <c r="E101" t="s">
+        <v>270</v>
+      </c>
+      <c r="F101" t="s">
+        <v>97</v>
+      </c>
+      <c r="G101" t="s">
+        <v>265</v>
+      </c>
+      <c r="H101" s="7">
+        <v>44138</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>14.641527999999999</v>
+      </c>
+      <c r="B102">
+        <v>-61.024174000000002</v>
+      </c>
+      <c r="C102">
+        <v>47</v>
+      </c>
+      <c r="D102">
+        <v>2</v>
+      </c>
+      <c r="E102" t="s">
+        <v>271</v>
+      </c>
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102" t="s">
+        <v>211</v>
+      </c>
+      <c r="H102" s="7">
+        <v>43954</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>12.238333000000001</v>
+      </c>
+      <c r="B103">
+        <v>-1.561593</v>
+      </c>
+      <c r="C103">
+        <v>47</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+      <c r="E103" t="s">
+        <v>229</v>
+      </c>
+      <c r="F103" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" t="s">
+        <v>211</v>
+      </c>
+      <c r="H103" s="7">
+        <v>44077</v>
+      </c>
+      <c r="I103" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>-4.0383329999999997</v>
+      </c>
+      <c r="B104">
+        <v>21.758664</v>
+      </c>
+      <c r="C104">
+        <v>50.833300000000001</v>
+      </c>
+      <c r="D104">
+        <v>4</v>
+      </c>
+      <c r="E104" t="s">
+        <v>273</v>
+      </c>
+      <c r="F104" t="s">
+        <v>7</v>
+      </c>
+      <c r="G104" t="s">
+        <v>211</v>
+      </c>
+      <c r="H104" s="7">
+        <v>44107</v>
+      </c>
+      <c r="I104" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>-26.522503</v>
+      </c>
+      <c r="B105">
+        <v>31.465865999999998</v>
+      </c>
+      <c r="C105">
+        <v>38.764600000000002</v>
+      </c>
+      <c r="D105">
+        <v>-95</v>
+      </c>
+      <c r="E105" t="s">
+        <v>275</v>
+      </c>
+      <c r="F105" t="s">
+        <v>97</v>
+      </c>
+      <c r="G105" t="s">
+        <v>265</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="I105" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>9.1449999999999996</v>
+      </c>
+      <c r="B106">
+        <v>40.489673000000003</v>
+      </c>
+      <c r="C106">
+        <v>36</v>
+      </c>
+      <c r="D106">
+        <v>138</v>
+      </c>
+      <c r="E106" t="s">
+        <v>278</v>
+      </c>
+      <c r="F106" t="s">
+        <v>94</v>
+      </c>
+      <c r="G106" t="s">
+        <v>212</v>
+      </c>
+      <c r="H106" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="I106" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>-0.80368899999999999</v>
+      </c>
+      <c r="B107">
+        <v>11.609444</v>
+      </c>
+      <c r="C107">
+        <v>47</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+      <c r="E107" t="s">
+        <v>281</v>
+      </c>
+      <c r="F107" t="s">
+        <v>13</v>
+      </c>
+      <c r="G107" t="s">
+        <v>211</v>
+      </c>
+      <c r="H107" s="7">
+        <v>44168</v>
+      </c>
+      <c r="I107" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>7.9465269999999997</v>
+      </c>
+      <c r="B108">
+        <v>-1.0231939999999999</v>
+      </c>
+      <c r="C108">
+        <v>60.472000000000001</v>
+      </c>
+      <c r="D108">
+        <v>8.4688999999999997</v>
+      </c>
+      <c r="E108" t="s">
+        <v>283</v>
+      </c>
+      <c r="F108" t="s">
+        <v>43</v>
+      </c>
+      <c r="G108" t="s">
+        <v>211</v>
+      </c>
+      <c r="H108" s="7">
+        <v>44168</v>
+      </c>
+      <c r="I108" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>9.9455869999999997</v>
+      </c>
+      <c r="B109">
+        <v>-9.6966450000000002</v>
+      </c>
+      <c r="C109">
+        <v>40</v>
+      </c>
+      <c r="D109">
+        <v>-4</v>
+      </c>
+      <c r="E109" t="s">
+        <v>217</v>
+      </c>
+      <c r="F109" t="s">
+        <v>48</v>
+      </c>
+      <c r="G109" t="s">
+        <v>211</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="I109" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>7.5399890000000003</v>
+      </c>
+      <c r="B110">
+        <v>-5.5470800000000002</v>
+      </c>
+      <c r="C110">
+        <v>43</v>
+      </c>
+      <c r="D110">
+        <v>12</v>
+      </c>
+      <c r="E110" t="s">
+        <v>286</v>
+      </c>
+      <c r="F110" t="s">
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
+        <v>0</v>
+      </c>
+      <c r="H110" s="7">
+        <v>44138</v>
+      </c>
+      <c r="I110" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>-2.3559E-2</v>
+      </c>
+      <c r="B111">
+        <v>37.906193000000002</v>
+      </c>
+      <c r="C111">
+        <v>38.764600000000002</v>
+      </c>
+      <c r="D111">
+        <v>-95</v>
+      </c>
+      <c r="E111" t="s">
+        <v>288</v>
+      </c>
+      <c r="F111" t="s">
+        <v>97</v>
+      </c>
+      <c r="G111" t="s">
+        <v>265</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="I111" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>21.00789</v>
+      </c>
+      <c r="B112">
+        <v>-10.940835</v>
+      </c>
+      <c r="C112">
+        <v>47</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="E112" t="s">
+        <v>290</v>
+      </c>
+      <c r="F112" t="s">
+        <v>13</v>
+      </c>
+      <c r="G112" t="s">
+        <v>211</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="I112" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>-22.957640000000001</v>
+      </c>
+      <c r="B113">
+        <v>18.490410000000001</v>
+      </c>
+      <c r="C113">
+        <v>40</v>
+      </c>
+      <c r="D113">
+        <v>-4</v>
+      </c>
+      <c r="E113" t="s">
+        <v>292</v>
+      </c>
+      <c r="F113" t="s">
+        <v>48</v>
+      </c>
+      <c r="G113" t="s">
+        <v>211</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="I113" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>-1.9402779999999999</v>
+      </c>
+      <c r="B114">
+        <v>29.873888000000001</v>
+      </c>
+      <c r="C114">
+        <v>21</v>
+      </c>
+      <c r="D114">
+        <v>78</v>
+      </c>
+      <c r="E114" t="s">
+        <v>294</v>
+      </c>
+      <c r="F114" t="s">
+        <v>110</v>
+      </c>
+      <c r="G114" t="s">
+        <v>212</v>
+      </c>
+      <c r="H114" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="I114" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>